<commit_message>
device OS & Friendly model
device OS & Friendly model names updated.
</commit_message>
<xml_diff>
--- a/Environment/TestLab.xlsx
+++ b/Environment/TestLab.xlsx
@@ -1,17 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27715"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pradeep/Documents/Test/MobileLabsAutomationFramework/Environment/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11760"/>
+    <workbookView xWindow="480" yWindow="460" windowWidth="28320" windowHeight="15240"/>
   </bookViews>
   <sheets>
     <sheet name="TestSet" sheetId="1" r:id="rId1"/>
     <sheet name="MultipleTestFolders" sheetId="9" r:id="rId2"/>
     <sheet name="Data" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -51,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="146">
   <si>
     <t>Build</t>
   </si>
@@ -158,12 +171,6 @@
     <t>UpsideDown</t>
   </si>
   <si>
-    <t>AndroidOS</t>
-  </si>
-  <si>
-    <t>iPhone OS</t>
-  </si>
-  <si>
     <t>deviceFriendlyModel</t>
   </si>
   <si>
@@ -194,15 +201,9 @@
     <t>iPad mini 3</t>
   </si>
   <si>
-    <t>iPhone 3GS</t>
-  </si>
-  <si>
     <t>iPhone 4</t>
   </si>
   <si>
-    <t>iPhone 4S</t>
-  </si>
-  <si>
     <t>iPhone 5</t>
   </si>
   <si>
@@ -224,9 +225,6 @@
     <t>iPod Touch 5G</t>
   </si>
   <si>
-    <t>iPod7,1</t>
-  </si>
-  <si>
     <t>Galaxy S3</t>
   </si>
   <si>
@@ -251,9 +249,6 @@
     <t>Nexus 7</t>
   </si>
   <si>
-    <t>Samsung Galaxy S6</t>
-  </si>
-  <si>
     <t>Galaxy Tab 2</t>
   </si>
   <si>
@@ -402,6 +397,111 @@
   </si>
   <si>
     <t>naveen.chauhan@mobilelabsinc.com</t>
+  </si>
+  <si>
+    <t>iOS</t>
+  </si>
+  <si>
+    <t>Android</t>
+  </si>
+  <si>
+    <t>iPhone 6s Plus</t>
+  </si>
+  <si>
+    <t>iPad Pro (9.7-inch)</t>
+  </si>
+  <si>
+    <t>HTC One E9s dual sim</t>
+  </si>
+  <si>
+    <t>iPod Touch 6G</t>
+  </si>
+  <si>
+    <t>iPad mini 4</t>
+  </si>
+  <si>
+    <t>Galaxy A5</t>
+  </si>
+  <si>
+    <t>Nexus 6P</t>
+  </si>
+  <si>
+    <t>Nexus 5X</t>
+  </si>
+  <si>
+    <t>Galaxy S7</t>
+  </si>
+  <si>
+    <t>Micromax Q424</t>
+  </si>
+  <si>
+    <t>Galaxy S6</t>
+  </si>
+  <si>
+    <t>iPhone 6s</t>
+  </si>
+  <si>
+    <t>iPad mini</t>
+  </si>
+  <si>
+    <t>SM-N920G</t>
+  </si>
+  <si>
+    <t>iPhone 7</t>
+  </si>
+  <si>
+    <t>SM-N910G</t>
+  </si>
+  <si>
+    <t>SM-T310</t>
+  </si>
+  <si>
+    <t>iPhone 7 Plus</t>
+  </si>
+  <si>
+    <t>ONE A2003</t>
+  </si>
+  <si>
+    <t>Galaxy S Captivate</t>
+  </si>
+  <si>
+    <t>LG-H918</t>
+  </si>
+  <si>
+    <t>Kindle Fire HD 8.9</t>
+  </si>
+  <si>
+    <t>iPhone 3Gs</t>
+  </si>
+  <si>
+    <t>SM-T350</t>
+  </si>
+  <si>
+    <t>GT-I9192</t>
+  </si>
+  <si>
+    <t>iPad Pro (12.9-inch)</t>
+  </si>
+  <si>
+    <t>LG-E980</t>
+  </si>
+  <si>
+    <t>iPad Pro</t>
+  </si>
+  <si>
+    <t>iPhone 4s</t>
+  </si>
+  <si>
+    <t>Galaxy S4 Mini</t>
+  </si>
+  <si>
+    <t>SM-G900H</t>
+  </si>
+  <si>
+    <t>ONE A2001</t>
+  </si>
+  <si>
+    <t>HTC One V</t>
   </si>
 </sst>
 </file>
@@ -475,16 +575,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -588,12 +688,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -623,12 +723,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -834,35 +934,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" style="12" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" style="12" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" style="12" customWidth="1"/>
-    <col min="9" max="9" width="24.28515625" style="12" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="12" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="12" customWidth="1"/>
-    <col min="12" max="12" width="17.140625" style="12" customWidth="1"/>
-    <col min="13" max="13" width="49.28515625" style="12" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" style="12" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" style="12" customWidth="1"/>
-    <col min="16" max="16" width="33.42578125" style="12" customWidth="1"/>
-    <col min="17" max="17" width="18.85546875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="12" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="17.5" style="12" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.5" style="12" customWidth="1"/>
+    <col min="9" max="9" width="24.33203125" style="12" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="12" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" style="12" customWidth="1"/>
+    <col min="12" max="12" width="17.1640625" style="12" customWidth="1"/>
+    <col min="13" max="13" width="49.33203125" style="12" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" style="12" customWidth="1"/>
+    <col min="15" max="15" width="12.5" style="12" customWidth="1"/>
+    <col min="16" max="16" width="33.5" style="12" customWidth="1"/>
+    <col min="17" max="17" width="18.83203125" style="12" customWidth="1"/>
     <col min="18" max="18" width="17" style="12" customWidth="1"/>
-    <col min="19" max="19" width="23.42578125" style="12" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="12"/>
+    <col min="19" max="19" width="23.5" style="12" customWidth="1"/>
+    <col min="20" max="16384" width="8.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="7" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -900,7 +1000,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>11</v>
@@ -912,54 +1012,54 @@
         <v>16</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="S1" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>105</v>
-      </c>
       <c r="H2" s="10" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>36</v>
+        <v>111</v>
       </c>
       <c r="L2" s="9">
         <v>9.3000000000000007</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="N2" s="9" t="s">
         <v>33</v>
@@ -971,13 +1071,13 @@
         <v>25</v>
       </c>
       <c r="Q2" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="S2" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -991,9 +1091,33 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Data!$B$2:$B$10</xm:f>
+            <xm:f>Data!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>P2:P1048576</xm:sqref>
+          <xm:sqref>K2:K1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Data!$F$2:$F$80</xm:f>
+          </x14:formula1>
+          <xm:sqref>J2:J1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Data!$I$2:$I$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q2:Q1048576 S2:S1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Data!$J$2:$J$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>R1:R1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Data!$G$2:$G$34</xm:f>
+          </x14:formula1>
+          <xm:sqref>M1:M1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -1009,33 +1133,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Data!$E$2:$E$3</xm:f>
+            <xm:f>Data!$B$2:$B$13</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Data!$F$2:$F$50</xm:f>
-          </x14:formula1>
-          <xm:sqref>J2:J1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Data!$I$2:$I$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>Q2:Q1048576 S2:S1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Data!$G$2:$G$25</xm:f>
-          </x14:formula1>
-          <xm:sqref>M1:M1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Data!$J$2:$J$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>R1:R1048576</xm:sqref>
+          <xm:sqref>P2:P1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1051,191 +1151,191 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="75.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="47.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="75.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1248,15 +1348,15 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Data!$B$2:$B$10</xm:f>
+            <xm:f>Data!$H$2:$H$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B1048576</xm:sqref>
+          <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Data!$H$2:$H$3</xm:f>
+            <xm:f>Data!$B$2:$B$13</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C1048576</xm:sqref>
+          <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1266,29 +1366,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="B9" sqref="B9:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="1"/>
-    <col min="9" max="9" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="40.42578125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="47.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="1"/>
+    <col min="9" max="9" width="17.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40.5" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1305,25 +1405,25 @@
         <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1337,28 +1437,28 @@
         <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>35</v>
+        <v>112</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="I2" s="1" t="b">
         <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1372,26 +1472,26 @@
         <v>50</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>36</v>
+        <v>111</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="I3" s="1" t="b">
         <v>0</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="K3" s="13"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1405,16 +1505,16 @@
         <v>75</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
@@ -1425,271 +1525,416 @@
         <v>100</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>68</v>
+        <v>118</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>70</v>
+        <v>132</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F11" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F12" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F13" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F14" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F15" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F16" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F17" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F18" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F19" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F20" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F21" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F22" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F23" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F24" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F25" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F26" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F27" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F28" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F29" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F30" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F31" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F32" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F33" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F34" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F35" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F36" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F37" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F38" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F39" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F40" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F41" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F42" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F43" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F44" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F45" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F46" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F47" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F48" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F49" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F50" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F51" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F52" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F53" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F54" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="55" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F55" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F56" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="57" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F57" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="58" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F58" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F59" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="60" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F60" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F61" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="62" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F62" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F63" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="64" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F64" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F65" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F66" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F11" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F12" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F13" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F14" s="1" t="s">
+    </row>
+    <row r="67" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F67" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="68" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F68" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F69" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="70" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F70" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="71" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F71" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="72" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F72" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="73" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F73" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="74" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F74" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="75" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F75" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="76" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F76" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="77" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F77" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F15" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F16" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F18" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F19" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F21" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F22" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F23" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F24" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F25" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F26" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F27" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F28" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F29" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F30" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F31" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F32" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F33" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F34" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F35" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F36" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F37" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F38" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F39" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F40" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="41" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F41" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="42" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F42" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="43" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F43" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="44" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F44" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="45" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F45" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="46" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F46" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="47" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F47" s="1" t="s">
+    <row r="78" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F78" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="79" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F79" s="1" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="48" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F48" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F49" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F50" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing from Shweta's end
Testing from Shweta's end
</commit_message>
<xml_diff>
--- a/Environment/TestLab.xlsx
+++ b/Environment/TestLab.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28908"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pradeep/Documents/Test/MobileLabsAutomationFramework/Environment/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="21600" windowHeight="9740"/>
   </bookViews>
@@ -18,11 +13,11 @@
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -747,7 +742,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -782,7 +777,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -994,10 +989,10 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="32.33203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="16.83203125" style="11" customWidth="1"/>
@@ -1021,7 +1016,7 @@
     <col min="20" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="7" customFormat="1" ht="15">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -1080,7 +1075,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19">
       <c r="A2" s="12" t="s">
         <v>162</v>
       </c>
@@ -1124,7 +1119,7 @@
         <v>33</v>
       </c>
       <c r="O2" s="8">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="P2" s="8" t="s">
         <v>28</v>
@@ -1145,7 +1140,7 @@
     <hyperlink ref="A2" r:id="rId2" display="7.5.6254.1201.master@db7c525"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
@@ -1199,6 +1194,9 @@
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
   </extLst>
 </worksheet>
 </file>
@@ -1211,7 +1209,7 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="64.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="75.5" style="2" bestFit="1" customWidth="1"/>
@@ -1219,7 +1217,7 @@
     <col min="4" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="4" customFormat="1" ht="15">
       <c r="A1" s="5" t="s">
         <v>84</v>
       </c>
@@ -1230,7 +1228,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>81</v>
       </c>
@@ -1239,7 +1237,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>82</v>
       </c>
@@ -1248,7 +1246,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>88</v>
       </c>
@@ -1257,7 +1255,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>134</v>
       </c>
@@ -1266,7 +1264,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>135</v>
       </c>
@@ -1277,7 +1275,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>136</v>
       </c>
@@ -1288,7 +1286,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>137</v>
       </c>
@@ -1299,7 +1297,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>138</v>
       </c>
@@ -1307,7 +1305,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>139</v>
       </c>
@@ -1318,7 +1316,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>140</v>
       </c>
@@ -1326,28 +1324,28 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>141</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>142</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
         <v>145</v>
       </c>
@@ -1356,55 +1354,55 @@
       </c>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
         <v>143</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
         <v>144</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" s="3"/>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1429,6 +1427,9 @@
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
   </extLst>
 </worksheet>
 </file>
@@ -1441,7 +1442,7 @@
       <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="74.83203125" style="1" bestFit="1" customWidth="1"/>
@@ -1457,7 +1458,7 @@
     <col min="12" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1492,7 +1493,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1525,7 +1526,7 @@
       </c>
       <c r="K2" s="12"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1558,7 +1559,7 @@
       </c>
       <c r="K3" s="12"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1581,7 +1582,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
@@ -1598,7 +1599,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="B6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1609,7 +1610,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1620,7 +1621,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
@@ -1631,7 +1632,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="B9" s="1" t="s">
         <v>28</v>
       </c>
@@ -1642,7 +1643,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1653,7 +1654,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="B11" s="1" t="s">
         <v>148</v>
       </c>
@@ -1664,7 +1665,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="B12" s="1" t="s">
         <v>149</v>
       </c>
@@ -1675,7 +1676,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="F13" s="1" t="s">
         <v>159</v>
       </c>
@@ -1683,7 +1684,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="F14" s="1" t="s">
         <v>157</v>
       </c>
@@ -1691,7 +1692,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="F15" s="1" t="s">
         <v>61</v>
       </c>
@@ -1699,7 +1700,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="F16" s="1" t="s">
         <v>54</v>
       </c>
@@ -1707,7 +1708,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="6:7">
       <c r="F17" s="1" t="s">
         <v>74</v>
       </c>
@@ -1715,7 +1716,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="6:7">
       <c r="F18" s="1" t="s">
         <v>70</v>
       </c>
@@ -1723,7 +1724,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="19" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="6:7">
       <c r="F19" s="1" t="s">
         <v>65</v>
       </c>
@@ -1731,352 +1732,352 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="6:7">
       <c r="F20" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="6:7">
       <c r="F21" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="6:7">
       <c r="F22" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="6:7">
       <c r="F23" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="6:7">
       <c r="F24" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="6:7">
       <c r="F25" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="6:7">
       <c r="F26" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="6:7">
       <c r="F27" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="6:7">
       <c r="F28" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="6:7">
       <c r="F29" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="6:7">
       <c r="F30" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="6:7">
       <c r="F31" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="6:7">
       <c r="F32" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="6:6">
       <c r="F33" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="6:6">
       <c r="F34" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="6:6">
       <c r="F35" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="6:6">
       <c r="F36" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="6:6">
       <c r="F37" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="6:6">
       <c r="F38" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="6:6">
       <c r="F39" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="40" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="6:6">
       <c r="F40" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="41" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="6:6">
       <c r="F41" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="42" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="6:6">
       <c r="F42" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="43" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="6:6">
       <c r="F43" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="6:6">
       <c r="F44" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="45" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="6:6">
       <c r="F45" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="6:6">
       <c r="F46" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="6:6">
       <c r="F47" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="6:6">
       <c r="F48" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="6:6">
       <c r="F49" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="6:6">
       <c r="F50" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="6:6">
       <c r="F51" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="6:6">
       <c r="F52" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="53" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="6:6">
       <c r="F53" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="54" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="6:6">
       <c r="F54" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="6:6">
       <c r="F55" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="6:6">
       <c r="F56" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="57" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="6:6">
       <c r="F57" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="58" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="6:6">
       <c r="F58" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="59" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="6:6">
       <c r="F59" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="60" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="6:6">
       <c r="F60" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="61" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="6:6">
       <c r="F61" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="62" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="6:6">
       <c r="F62" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="63" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="6:6">
       <c r="F63" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="6:6">
       <c r="F64" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="6:6">
       <c r="F65" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="6:6">
       <c r="F66" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="6:6">
       <c r="F67" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="6:6">
       <c r="F68" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="69" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="6:6">
       <c r="F69" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="70" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="6:6">
       <c r="F70" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="6:6">
       <c r="F71" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="72" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="6:6">
       <c r="F72" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="73" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="6:6">
       <c r="F73" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="74" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="6:6">
       <c r="F74" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="75" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="6:6">
       <c r="F75" s="1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="76" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="6:6">
       <c r="F76" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="6:6">
       <c r="F77" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="78" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="6:6">
       <c r="F78" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="79" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="6:6">
       <c r="F79" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="80" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="6:6">
       <c r="F80" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="81" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="6:6">
       <c r="F81" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="82" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="6:6">
       <c r="F82" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="83" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="6:6">
       <c r="F83" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="84" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="6:6">
       <c r="F84" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="85" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="6:6">
       <c r="F85" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="86" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="6:6">
       <c r="F86" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="87" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="6:6">
       <c r="F87" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="88" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="6:6">
       <c r="F88" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="89" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="6:6">
       <c r="F89" s="1" t="s">
         <v>79</v>
       </c>
@@ -2086,6 +2087,11 @@
     <sortCondition ref="G2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>